<commit_message>
fixed Getting WB Data
</commit_message>
<xml_diff>
--- a/WB_data/Selected_Indicators.xlsx
+++ b/WB_data/Selected_Indicators.xlsx
@@ -60,7 +60,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -75,11 +75,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
     </font>
     <font>
       <u/>
@@ -98,11 +93,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Consolas"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
@@ -117,7 +107,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -140,36 +130,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -456,11 +430,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -469,7 +441,7 @@
     <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,7 +452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -490,10 +462,9 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
@@ -502,258 +473,6 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
-      <c r="B35" s="3"/>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F49" s="1"/>
-    </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F51" s="1"/>
-    </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F57" s="2"/>
-    </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F59" s="1"/>
-    </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F60" s="1"/>
-    </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F62" s="1"/>
-    </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F63" s="1"/>
-    </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F64" s="1"/>
-    </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F65" s="1"/>
-    </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F66" s="1"/>
-    </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F67" s="1"/>
-    </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F68" s="1"/>
-    </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F69" s="1"/>
-    </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F70" s="1"/>
-    </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F71" s="1"/>
-    </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F72" s="1"/>
-    </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F73" s="1"/>
-    </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F75" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>